<commit_message>
running version of CRS_BRS_SIM
</commit_message>
<xml_diff>
--- a/CRS_BRS_SIM/input.xlsx
+++ b/CRS_BRS_SIM/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanneshenglein/Desktop/Masterarbeit/VehicleOemofIntegration/Erster_Test_KOMBI_DES(MB+Car_MB)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B87DD6-9302-B244-958D-00877C9AE1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8439665B-CF56-6B4F-9411-54A3299CC704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="15980" xr2:uid="{77293274-C4CB-421E-9B2C-ED6957626F24}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15980" xr2:uid="{77293274-C4CB-421E-9B2C-ED6957626F24}"/>
   </bookViews>
   <sheets>
     <sheet name="general_settings" sheetId="7" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
   <si>
     <t>[d]</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Capacity of SimPy Store aka total number of cars</t>
   </si>
   <si>
-    <t>Daily trip demand, is the ex ante generated number of trips per day</t>
-  </si>
-  <si>
     <t>simulated_days</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>standart deviation "evening departure"</t>
   </si>
   <si>
-    <t>mean value " vening departure"</t>
-  </si>
-  <si>
     <t>standart deviation "morning departure"</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>BRS_energycontent</t>
   </si>
   <si>
-    <t>Wh</t>
-  </si>
-  <si>
     <t>Energy content of one MB in Wh</t>
   </si>
   <si>
@@ -183,157 +174,181 @@
     <t>trigger for enabeling range extending CRS with MB</t>
   </si>
   <si>
+    <t>medical_Cooling</t>
+  </si>
+  <si>
+    <t>Car properties setup</t>
+  </si>
+  <si>
+    <t>energy_consumption</t>
+  </si>
+  <si>
+    <t>avg_velocity</t>
+  </si>
+  <si>
+    <t>[Wh/km]</t>
+  </si>
+  <si>
+    <t>[km/h]</t>
+  </si>
+  <si>
+    <t>energy consumed per kilometer travelled (aCar)</t>
+  </si>
+  <si>
+    <t>average velocity of cars (in SSA)</t>
+  </si>
+  <si>
+    <t>Trip departure probability setup</t>
+  </si>
+  <si>
+    <t>Trip lenght probability setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean value of the underlying normal distribution. </t>
+  </si>
+  <si>
+    <t>Standard deviation of the underlying normal distribution</t>
+  </si>
+  <si>
+    <t>[km]</t>
+  </si>
+  <si>
+    <t>mu_trip_length</t>
+  </si>
+  <si>
+    <t>sigma_trip_length</t>
+  </si>
+  <si>
+    <t>Trip extra time probability setup</t>
+  </si>
+  <si>
+    <t>min_return_soc</t>
+  </si>
+  <si>
+    <t>min return SOC of car</t>
+  </si>
+  <si>
+    <t>fix_bat_size</t>
+  </si>
+  <si>
+    <t>Energycontent of the fixed battery of the car</t>
+  </si>
+  <si>
+    <t>mu_idle_time</t>
+  </si>
+  <si>
+    <t>sigma_idle_time</t>
+  </si>
+  <si>
+    <t>REX Request Setup</t>
+  </si>
+  <si>
+    <t>REX_patience</t>
+  </si>
+  <si>
+    <t>time a trip waits to get MB for REX</t>
+  </si>
+  <si>
+    <t>leaving SOC of a car, Oemof charges car to that SOC level before each trip</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>debug</t>
+  </si>
+  <si>
+    <t>trigger for enabeling debug printing</t>
+  </si>
+  <si>
+    <t>mu_daily_CRS_trip_demand</t>
+  </si>
+  <si>
+    <t>mu_daily_BRS_rental_demand</t>
+  </si>
+  <si>
+    <t>BRS Fleet Setup</t>
+  </si>
+  <si>
+    <t>MB Request Setup</t>
+  </si>
+  <si>
+    <t>MB properties setup</t>
+  </si>
+  <si>
+    <t>mobile_Lighting</t>
+  </si>
+  <si>
+    <t>PUE_Cooling</t>
+  </si>
+  <si>
+    <t>eVBS_Water</t>
+  </si>
+  <si>
+    <t>eVBS_Fire</t>
+  </si>
+  <si>
+    <t>PUE_Milling</t>
+  </si>
+  <si>
+    <t>PUE_Cocoa</t>
+  </si>
+  <si>
+    <t>PUE_Welding</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>Household</t>
+  </si>
+  <si>
+    <t>electric_Fishing</t>
+  </si>
+  <si>
     <t>False</t>
   </si>
   <si>
-    <t>medical_Cooling</t>
-  </si>
-  <si>
-    <t>daily_CRS_trip_demand</t>
-  </si>
-  <si>
-    <t>Daily trip demand, is the ex ante generated number of MB rental requests per day</t>
-  </si>
-  <si>
-    <t>daily_BRS_rental_demand</t>
-  </si>
-  <si>
-    <t>Car properties setup</t>
-  </si>
-  <si>
-    <t>energy_consumption</t>
-  </si>
-  <si>
-    <t>avg_velocity</t>
-  </si>
-  <si>
-    <t>[Wh/km]</t>
-  </si>
-  <si>
-    <t>[km/h]</t>
-  </si>
-  <si>
-    <t>energy consumed per kilometer travelled (aCar)</t>
-  </si>
-  <si>
-    <t>average velocity of cars (in SSA)</t>
-  </si>
-  <si>
-    <t>Trip departure probability setup</t>
-  </si>
-  <si>
-    <t>Trip lenght probability setup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean value of the underlying normal distribution. </t>
-  </si>
-  <si>
-    <t>Standard deviation of the underlying normal distribution</t>
-  </si>
-  <si>
-    <t>[km]</t>
-  </si>
-  <si>
-    <t>mu_trip_length</t>
-  </si>
-  <si>
-    <t>sigma_trip_length</t>
-  </si>
-  <si>
-    <t>Trip extra time probability setup</t>
-  </si>
-  <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>min_return_soc</t>
-  </si>
-  <si>
-    <t>min return SOC of car</t>
-  </si>
-  <si>
-    <t>fix_bat_size</t>
-  </si>
-  <si>
-    <t>Energycontent of the fixed battery of the car</t>
-  </si>
-  <si>
-    <t>mu_idle_time</t>
-  </si>
-  <si>
-    <t>sigma_idle_time</t>
-  </si>
-  <si>
-    <t>REX Request Setup</t>
-  </si>
-  <si>
-    <t>REX_patience</t>
-  </si>
-  <si>
-    <t>time a trip waits to get MB for REX</t>
-  </si>
-  <si>
-    <t>leaving SOC of a car, Oemof charges car to that SOC level before each trip</t>
-  </si>
-  <si>
-    <t>CRS_leaving_SOC</t>
-  </si>
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>debug</t>
-  </si>
-  <si>
-    <t>trigger for enabeling debug printing</t>
-  </si>
-  <si>
-    <t>mu_daily_CRS_trip_demand</t>
-  </si>
-  <si>
-    <t>mu_daily_BRS_rental_demand</t>
-  </si>
-  <si>
-    <t>BRS Fleet Setup</t>
-  </si>
-  <si>
-    <t>MB Request Setup</t>
-  </si>
-  <si>
-    <t>MB properties setup</t>
-  </si>
-  <si>
-    <t>mobile_Lighting</t>
-  </si>
-  <si>
-    <t>PUE_Cooling</t>
-  </si>
-  <si>
-    <t>eVBS_Water</t>
-  </si>
-  <si>
-    <t>eVBS_Fire</t>
-  </si>
-  <si>
-    <t>PUE_Milling</t>
-  </si>
-  <si>
-    <t>PUE_Cocoa</t>
-  </si>
-  <si>
-    <t>PUE_Hilit</t>
-  </si>
-  <si>
-    <t>PUE_Welding</t>
-  </si>
-  <si>
-    <t>Party</t>
-  </si>
-  <si>
-    <t>Household</t>
-  </si>
-  <si>
-    <t>electric_Fishing</t>
+    <t>sigma_daily_CRS_trip_demand</t>
+  </si>
+  <si>
+    <t>mean Daily trip demand, is the ex ante generated number of trips per day</t>
+  </si>
+  <si>
+    <t>standart deviation CRS trip demand</t>
+  </si>
+  <si>
+    <t>sigma_daily_BRS_rental_demand</t>
+  </si>
+  <si>
+    <t>Daily rental demand, is the ex ante generated number of MB rental requests per day</t>
+  </si>
+  <si>
+    <t>[W]</t>
+  </si>
+  <si>
+    <t>CRS_charge_power</t>
+  </si>
+  <si>
+    <t>BRS_charge_power</t>
+  </si>
+  <si>
+    <t>charging power for one car, used to determine "charge time"</t>
+  </si>
+  <si>
+    <t>charging power for one MB, used to determine "charge time"</t>
+  </si>
+  <si>
+    <t>PUE_Hilti</t>
+  </si>
+  <si>
+    <t>mean value " evening departure"</t>
+  </si>
+  <si>
+    <t>[h]</t>
+  </si>
+  <si>
+    <t>CRS_leaving_soc</t>
   </si>
 </sst>
 </file>
@@ -400,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -421,10 +436,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -744,7 +755,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -756,7 +767,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -764,49 +775,49 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
         <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -814,35 +825,35 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="5">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -850,16 +861,16 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -879,10 +890,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF08339-FC61-6448-9C1E-448A2FA5E0F3}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:D20"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -894,7 +905,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -902,13 +913,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -916,7 +927,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -924,40 +935,49 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>87</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -965,21 +985,21 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -987,51 +1007,63 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
+      <c r="C10" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
+      <c r="C11" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>17</v>
       </c>
+      <c r="C12" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
+      <c r="C13" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1039,35 +1071,35 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B15">
         <v>3.2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B16">
         <v>0.88</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1075,35 +1107,35 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1111,7 +1143,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B21" s="3">
         <v>30000</v>
@@ -1120,63 +1152,77 @@
         <v>1</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <v>300</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B23">
         <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B24">
         <v>0.05</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26">
+        <v>11000</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1187,19 +1233,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9425BC48-D58E-0541-A07C-4CABF733DC39}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0"/>
+    <sheetView zoomScale="173" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1207,21 +1255,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1229,39 +1277,42 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>81</v>
+        <v>90</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1269,16 +1320,30 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>2000</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1291,7 +1356,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="169" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1303,24 +1368,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>85</v>
+      <c r="A2" t="s">
+        <v>76</v>
       </c>
       <c r="B2">
         <v>18</v>
@@ -1328,7 +1393,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="9">
         <v>420</v>
       </c>
       <c r="E2">
@@ -1336,8 +1401,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>13</v>
+      <c r="A3" t="s">
+        <v>12</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -1345,7 +1410,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>84</v>
       </c>
       <c r="E3">
@@ -1353,8 +1418,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>46</v>
+      <c r="A4" t="s">
+        <v>42</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -1362,7 +1427,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>76</v>
       </c>
       <c r="E4">
@@ -1370,8 +1435,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>86</v>
+      <c r="A5" t="s">
+        <v>77</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -1379,7 +1444,7 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>75</v>
       </c>
       <c r="E5">
@@ -1387,8 +1452,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>87</v>
+      <c r="A6" t="s">
+        <v>78</v>
       </c>
       <c r="B6">
         <v>8</v>
@@ -1396,7 +1461,7 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>110</v>
       </c>
       <c r="E6">
@@ -1404,8 +1469,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>88</v>
+      <c r="A7" t="s">
+        <v>79</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -1413,7 +1478,7 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <v>1100</v>
       </c>
       <c r="E7">
@@ -1421,8 +1486,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>89</v>
+      <c r="A8" t="s">
+        <v>80</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -1430,7 +1495,7 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>750</v>
       </c>
       <c r="E8">
@@ -1438,8 +1503,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>90</v>
+      <c r="A9" t="s">
+        <v>81</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1447,7 +1512,7 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <v>1850</v>
       </c>
       <c r="E9">
@@ -1455,8 +1520,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>91</v>
+      <c r="A10" t="s">
+        <v>97</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1464,7 +1529,7 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <v>650</v>
       </c>
       <c r="E10">
@@ -1472,8 +1537,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>92</v>
+      <c r="A11" t="s">
+        <v>82</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -1481,7 +1546,7 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <v>400</v>
       </c>
       <c r="E11">
@@ -1489,8 +1554,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>93</v>
+      <c r="A12" t="s">
+        <v>83</v>
       </c>
       <c r="B12">
         <v>18</v>
@@ -1498,7 +1563,7 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <v>2000</v>
       </c>
       <c r="E12">
@@ -1506,8 +1571,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>94</v>
+      <c r="A13" t="s">
+        <v>84</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1515,7 +1580,7 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <v>10</v>
       </c>
       <c r="E13">
@@ -1523,8 +1588,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>95</v>
+      <c r="A14" t="s">
+        <v>85</v>
       </c>
       <c r="B14">
         <v>18</v>
@@ -1532,7 +1597,7 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>1092</v>
       </c>
       <c r="E14">

</xml_diff>